<commit_message>
Update use case schema, make all
</commit_message>
<xml_diff>
--- a/project/excel/standards_usecase_schema.xlsx
+++ b/project/excel/standards_usecase_schema.xlsx
@@ -454,7 +454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,32 +480,78 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>UseCase_primary_email</t>
+          <t>use_case_category</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>known_limitations</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>age_in_years</t>
+          <t>relevance_to_dgps</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>vital_status</t>
+          <t>data_types</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>data_substrates</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>standards_and_tools_for_dgp_use</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>alternative_standards_and_tools</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>enables</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>involved_in_experimental_design</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>involved_in_metadata_management</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>involved_in_quality_control</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>xrefs</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation sqref="G2:G1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>"ALIVE,DEAD,UNKNOWN"</formula1>
+  <dataValidations count="4">
+    <dataValidation sqref="D2:D1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Acquisition,Integration,Standardization,Modeling,Application,Assessment"</formula1>
     </dataValidation>
-    <dataValidation sqref="G2:G1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>"ALIVE,DEAD,UNKNOWN"</formula1>
+    <dataValidation sqref="F2:F1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"AI-READI,CHoRUS,CM4AI,Voice"</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"Acquisition,Integration,Standardization,Modeling,Application,Assessment"</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
+      <formula1>"AI-READI,CHoRUS,CM4AI,Voice"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -580,7 +626,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -606,22 +652,62 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>UseCase_primary_email</t>
+          <t>use_case_category</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>known_limitations</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>age_in_years</t>
+          <t>relevance_to_dgps</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>vital_status</t>
+          <t>data_types</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>data_substrates</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>standards_and_tools_for_dgp_use</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>alternative_standards_and_tools</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>enables</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>involved_in_experimental_design</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>involved_in_metadata_management</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>involved_in_quality_control</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>xrefs</t>
         </is>
       </c>
     </row>

</xml_diff>